<commit_message>
add code for importing retirement rate for male class AB members.
</commit_message>
<xml_diff>
--- a/Data/TPAF Cenus Data.xlsx
+++ b/Data/TPAF Cenus Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="656" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="656" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="39">
   <si>
     <t>Table of Contents</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>35-39</t>
+  </si>
+  <si>
+    <t>40&amp;up</t>
   </si>
   <si>
     <t>Total</t>
@@ -213,16 +216,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -294,8 +293,8 @@
   </sheetPr>
   <dimension ref="A2:L14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L20" activeCellId="0" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -331,14 +330,14 @@
       <c r="I2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="0" t="n">
-        <v>40</v>
+      <c r="J2" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -533,7 +532,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>369</v>
@@ -571,7 +570,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>227</v>
@@ -609,7 +608,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>209</v>
@@ -647,7 +646,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>152</v>
@@ -685,7 +684,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>106</v>
@@ -723,7 +722,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>15</v>
@@ -761,7 +760,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>5025</v>
@@ -812,8 +811,8 @@
   </sheetPr>
   <dimension ref="A2:L14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -853,10 +852,10 @@
         <v>40</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -893,7 +892,7 @@
       <c r="K3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L3" s="2" t="n">
+      <c r="L3" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -931,7 +930,7 @@
       <c r="K4" s="0" t="n">
         <v>1135</v>
       </c>
-      <c r="L4" s="2" t="n">
+      <c r="L4" s="0" t="n">
         <v>50629</v>
       </c>
     </row>
@@ -969,7 +968,7 @@
       <c r="K5" s="0" t="n">
         <v>10719</v>
       </c>
-      <c r="L5" s="2" t="n">
+      <c r="L5" s="0" t="n">
         <v>52685</v>
       </c>
     </row>
@@ -1007,7 +1006,7 @@
       <c r="K6" s="0" t="n">
         <v>15558</v>
       </c>
-      <c r="L6" s="2" t="n">
+      <c r="L6" s="0" t="n">
         <v>58051</v>
       </c>
     </row>
@@ -1045,13 +1044,13 @@
       <c r="K7" s="0" t="n">
         <v>14592</v>
       </c>
-      <c r="L7" s="2" t="n">
+      <c r="L7" s="0" t="n">
         <v>65367</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1512</v>
@@ -1083,13 +1082,13 @@
       <c r="K8" s="0" t="n">
         <v>13751</v>
       </c>
-      <c r="L8" s="2" t="n">
+      <c r="L8" s="0" t="n">
         <v>71799</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1171</v>
@@ -1121,13 +1120,13 @@
       <c r="K9" s="0" t="n">
         <v>11420</v>
       </c>
-      <c r="L9" s="2" t="n">
+      <c r="L9" s="0" t="n">
         <v>74606</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>695</v>
@@ -1159,13 +1158,13 @@
       <c r="K10" s="0" t="n">
         <v>12342</v>
       </c>
-      <c r="L10" s="2" t="n">
+      <c r="L10" s="0" t="n">
         <v>77593</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>395</v>
@@ -1197,13 +1196,13 @@
       <c r="K11" s="0" t="n">
         <v>13591</v>
       </c>
-      <c r="L11" s="2" t="n">
+      <c r="L11" s="0" t="n">
         <v>81507</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>149</v>
@@ -1235,13 +1234,13 @@
       <c r="K12" s="0" t="n">
         <v>10082</v>
       </c>
-      <c r="L12" s="2" t="n">
+      <c r="L12" s="0" t="n">
         <v>86694</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>31</v>
@@ -1273,13 +1272,13 @@
       <c r="K13" s="0" t="n">
         <v>3228</v>
       </c>
-      <c r="L13" s="2" t="n">
+      <c r="L13" s="0" t="n">
         <v>88797</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>17784</v>
@@ -1311,7 +1310,6 @@
       <c r="K14" s="0" t="n">
         <v>106418</v>
       </c>
-      <c r="L14" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1372,10 +1370,10 @@
         <v>40</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1570,7 +1568,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>90</v>
@@ -1608,7 +1606,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>59</v>
@@ -1646,7 +1644,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>82</v>
@@ -1684,7 +1682,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>54</v>
@@ -1722,7 +1720,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>52</v>
@@ -1759,8 +1757,8 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>18</v>
+      <c r="A13" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>139</v>
@@ -1798,7 +1796,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>982</v>
@@ -1890,10 +1888,10 @@
         <v>40</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2088,7 +2086,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>313</v>
@@ -2126,7 +2124,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>276</v>
@@ -2164,7 +2162,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>226</v>
@@ -2202,7 +2200,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>197</v>
@@ -2240,7 +2238,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>127</v>
@@ -2278,7 +2276,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>199</v>
@@ -2316,7 +2314,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>3481</v>
@@ -2382,69 +2380,69 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="E4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="G4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="n">
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="0" t="n">
         <v>9168</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="0" t="n">
         <v>9168</v>
       </c>
     </row>
@@ -2455,157 +2453,157 @@
       <c r="B6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="0" t="n">
         <v>22092</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="0" t="n">
         <v>38580</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="0" t="n">
         <v>60672</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="0" t="n">
         <v>80568</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="0" t="n">
         <v>225984</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="0" t="n">
         <v>306552</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="0" t="n">
         <v>62616</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="0" t="n">
         <v>452808</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="0" t="n">
         <v>515424</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="0" t="n">
         <v>228012</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="E9" s="0" t="n">
         <v>492276</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="0" t="n">
         <v>720288</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="0" t="n">
         <v>278424</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="0" t="n">
         <v>141</v>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="0" t="n">
         <v>1979592</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="0" t="n">
         <v>162</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="0" t="n">
         <v>2258016</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" s="0" t="n">
         <v>155040</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="0" t="n">
         <v>68</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="E11" s="0" t="n">
         <v>1048200</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="0" t="n">
         <v>79</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="0" t="n">
         <v>1203240</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="C12" s="0" t="n">
         <v>826752</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="0" t="n">
         <v>298</v>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="0" t="n">
         <v>4246608</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="0" t="n">
         <v>351</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="0" t="n">
         <v>5073360</v>
       </c>
     </row>
@@ -2644,345 +2642,345 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="E4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="G4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="0" t="n">
         <v>58206</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="0" t="n">
         <v>257471</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="3" t="n">
         <v>315677</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="0" t="n">
         <v>2060968</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>175</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="0" t="n">
         <v>5655493</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>230</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="3" t="n">
         <v>7716461</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>692</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="0" t="n">
         <v>34255299</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>2243</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="0" t="n">
         <v>100423739</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>2935</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="3" t="n">
         <v>134679038</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>3982</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="0" t="n">
         <v>197380850</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>11095</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="0" t="n">
         <v>476523377</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>15077</v>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="G8" s="3" t="n">
         <v>673904227</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>7713</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="0" t="n">
         <v>373763921</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>16045</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="E9" s="0" t="n">
         <v>661739099</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>23758</v>
       </c>
-      <c r="G9" s="4" t="n">
+      <c r="G9" s="3" t="n">
         <v>1035503020</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>5700</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="0" t="n">
         <v>264802956</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>10603</v>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="0" t="n">
         <v>407527707</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>16303</v>
       </c>
-      <c r="G10" s="4" t="n">
+      <c r="G10" s="3" t="n">
         <v>672330663</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>3520</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" s="0" t="n">
         <v>156727913</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>6352</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="E11" s="0" t="n">
         <v>226309980</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>9872</v>
       </c>
-      <c r="G11" s="4" t="n">
+      <c r="G11" s="3" t="n">
         <v>383037893</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>2804</v>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="C12" s="0" t="n">
         <v>115313668</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>4807</v>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="0" t="n">
         <v>152101000</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>7611</v>
       </c>
-      <c r="G12" s="4" t="n">
+      <c r="G12" s="3" t="n">
         <v>267414668</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1515</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C13" s="0" t="n">
         <v>53519096</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>3260</v>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="0" t="n">
         <v>83513848</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>4775</v>
       </c>
-      <c r="G13" s="4" t="n">
+      <c r="G13" s="3" t="n">
         <v>137032944</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>487</v>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="C14" s="0" t="n">
         <v>13936304</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>1521</v>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="0" t="n">
         <v>32570420</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>2008</v>
       </c>
-      <c r="G14" s="4" t="n">
+      <c r="G14" s="3" t="n">
         <v>46506724</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>87</v>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C15" s="0" t="n">
         <v>2081972</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>485</v>
       </c>
-      <c r="E15" s="2" t="n">
+      <c r="E15" s="0" t="n">
         <v>9129041</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>572</v>
       </c>
-      <c r="G15" s="4" t="n">
+      <c r="G15" s="3" t="n">
         <v>11211013</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="C16" s="2" t="n">
+      <c r="C16" s="0" t="n">
         <v>154212</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>101</v>
       </c>
-      <c r="E16" s="2" t="n">
+      <c r="E16" s="0" t="n">
         <v>1880607</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>108</v>
       </c>
-      <c r="G16" s="4" t="n">
+      <c r="G16" s="3" t="n">
         <v>2034819</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>26564</v>
       </c>
-      <c r="C17" s="2" t="n">
+      <c r="C17" s="0" t="n">
         <v>1214055365</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>56701</v>
       </c>
-      <c r="E17" s="2" t="n">
+      <c r="E17" s="0" t="n">
         <v>2157631782</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>83265</v>
       </c>
-      <c r="G17" s="4" t="n">
+      <c r="G17" s="3" t="n">
         <v>3371687147</v>
       </c>
     </row>
@@ -3005,7 +3003,7 @@
   <dimension ref="A2:G17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3021,69 +3019,69 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="E4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="G4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="B5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="0" t="n">
         <v>36624</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="0" t="n">
         <v>20951</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="0" t="n">
         <v>57575</v>
       </c>
     </row>
@@ -3091,275 +3089,275 @@
       <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="0" t="n">
         <v>53256</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="0" t="n">
         <v>336256</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="0" t="n">
         <v>389512</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="0" t="n">
         <v>231348</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="0" t="n">
         <v>717302</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="0" t="n">
         <v>948650</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="0" t="n">
         <v>530162</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="0" t="n">
         <v>72</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="0" t="n">
         <v>1950917</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="0" t="n">
         <v>89</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="0" t="n">
         <v>2481079</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="0" t="n">
         <v>772624</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="0" t="n">
         <v>153</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="E9" s="0" t="n">
         <v>4501727</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="0" t="n">
         <v>181</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="0" t="n">
         <v>5274351</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B10" s="0" t="n">
         <v>76</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="0" t="n">
         <v>2202977</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="0" t="n">
         <v>282</v>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="0" t="n">
         <v>8456961</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="0" t="n">
         <v>358</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="0" t="n">
         <v>10659938</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B11" s="0" t="n">
         <v>142</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" s="0" t="n">
         <v>4185824</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="0" t="n">
         <v>511</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="E11" s="0" t="n">
         <v>14741015</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="0" t="n">
         <v>653</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="0" t="n">
         <v>18926839</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="B12" s="0" t="n">
         <v>189</v>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="C12" s="0" t="n">
         <v>5544757</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="0" t="n">
         <v>534</v>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="0" t="n">
         <v>15495538</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="0" t="n">
         <v>723</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="0" t="n">
         <v>21040295</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="B13" s="0" t="n">
         <v>96</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C13" s="0" t="n">
         <v>2535157</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="0" t="n">
         <v>388</v>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="0" t="n">
         <v>10525698</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="0" t="n">
         <v>484</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="0" t="n">
         <v>13060855</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="B14" s="0" t="n">
         <v>68</v>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="C14" s="0" t="n">
         <v>1781867</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="0" t="n">
         <v>220</v>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="0" t="n">
         <v>5638245</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="0" t="n">
         <v>288</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="0" t="n">
         <v>7420112</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="B15" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C15" s="0" t="n">
         <v>708164</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D15" s="0" t="n">
         <v>115</v>
       </c>
-      <c r="E15" s="2" t="n">
+      <c r="E15" s="0" t="n">
         <v>2411466</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="0" t="n">
         <v>149</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="0" t="n">
         <v>3119630</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="B16" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="C16" s="2" t="n">
+      <c r="C16" s="0" t="n">
         <v>336317</v>
       </c>
-      <c r="D16" s="2" t="n">
+      <c r="D16" s="0" t="n">
         <v>86</v>
       </c>
-      <c r="E16" s="2" t="n">
+      <c r="E16" s="0" t="n">
         <v>1571798</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="0" t="n">
         <v>104</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G16" s="0" t="n">
         <v>1908115</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B17" s="0" t="n">
         <v>680</v>
       </c>
-      <c r="C17" s="2" t="n">
+      <c r="C17" s="0" t="n">
         <v>18919077</v>
       </c>
-      <c r="D17" s="2" t="n">
+      <c r="D17" s="0" t="n">
         <v>2405</v>
       </c>
-      <c r="E17" s="2" t="n">
+      <c r="E17" s="0" t="n">
         <v>66367874</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="0" t="n">
         <v>3085</v>
       </c>
-      <c r="G17" s="2" t="n">
+      <c r="G17" s="0" t="n">
         <v>85286951</v>
       </c>
     </row>
@@ -3392,69 +3390,69 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="E4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="G4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="B5" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="0" t="n">
         <v>77078</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="0" t="n">
         <v>58103</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="0" t="n">
         <v>135181</v>
       </c>
     </row>
@@ -3462,22 +3460,22 @@
       <c r="A6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="0" t="n">
         <v>81780</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="0" t="n">
         <v>73045</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="0" t="n">
         <v>154825</v>
       </c>
     </row>
@@ -3485,22 +3483,22 @@
       <c r="A7" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="0" t="n">
         <v>91421</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="0" t="n">
         <v>103166</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="0" t="n">
         <v>194587</v>
       </c>
     </row>
@@ -3508,344 +3506,344 @@
       <c r="A8" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="0" t="n">
         <v>50869</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="0" t="n">
         <v>218984</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="0" t="n">
         <v>269853</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B9" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="0" t="n">
         <v>280522</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="E9" s="0" t="n">
         <v>433271</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="0" t="n">
         <v>713793</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B10" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="0" t="n">
         <v>416108</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="0" t="n">
         <v>528170</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="0" t="n">
         <v>944278</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B11" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" s="0" t="n">
         <v>450369</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="E11" s="0" t="n">
         <v>1040333</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="0" t="n">
         <v>76</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="0" t="n">
         <v>1490702</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B12" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="C12" s="0" t="n">
         <v>1453142</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="0" t="n">
         <v>107</v>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="0" t="n">
         <v>2775389</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="0" t="n">
         <v>165</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="0" t="n">
         <v>4228531</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B13" s="0" t="n">
         <v>168</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C13" s="0" t="n">
         <v>4114146</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="0" t="n">
         <v>296</v>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="0" t="n">
         <v>8455817</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="0" t="n">
         <v>464</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="0" t="n">
         <v>12569963</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="B14" s="0" t="n">
         <v>295</v>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="C14" s="0" t="n">
         <v>7421160</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="0" t="n">
         <v>452</v>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="0" t="n">
         <v>14031323</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="0" t="n">
         <v>747</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="0" t="n">
         <v>21452483</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="B15" s="0" t="n">
         <v>204</v>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C15" s="0" t="n">
         <v>4847851</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D15" s="0" t="n">
         <v>584</v>
       </c>
-      <c r="E15" s="2" t="n">
+      <c r="E15" s="0" t="n">
         <v>17121333</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="0" t="n">
         <v>788</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="0" t="n">
         <v>21969184</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="B16" s="0" t="n">
         <v>198</v>
       </c>
-      <c r="C16" s="2" t="n">
+      <c r="C16" s="0" t="n">
         <v>4620339</v>
       </c>
-      <c r="D16" s="2" t="n">
+      <c r="D16" s="0" t="n">
         <v>702</v>
       </c>
-      <c r="E16" s="2" t="n">
+      <c r="E16" s="0" t="n">
         <v>19749128</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="0" t="n">
         <v>900</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G16" s="0" t="n">
         <v>24369467</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="B17" s="0" t="n">
         <v>156</v>
       </c>
-      <c r="C17" s="2" t="n">
+      <c r="C17" s="0" t="n">
         <v>3189233</v>
       </c>
-      <c r="D17" s="2" t="n">
+      <c r="D17" s="0" t="n">
         <v>694</v>
       </c>
-      <c r="E17" s="2" t="n">
+      <c r="E17" s="0" t="n">
         <v>18727568</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="0" t="n">
         <v>850</v>
       </c>
-      <c r="G17" s="2" t="n">
+      <c r="G17" s="0" t="n">
         <v>21916801</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="B18" s="0" t="n">
         <v>113</v>
       </c>
-      <c r="C18" s="2" t="n">
+      <c r="C18" s="0" t="n">
         <v>1918968</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="D18" s="0" t="n">
         <v>595</v>
       </c>
-      <c r="E18" s="2" t="n">
+      <c r="E18" s="0" t="n">
         <v>13065679</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="0" t="n">
         <v>708</v>
       </c>
-      <c r="G18" s="2" t="n">
+      <c r="G18" s="0" t="n">
         <v>14984647</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="B19" s="0" t="n">
         <v>61</v>
       </c>
-      <c r="C19" s="2" t="n">
+      <c r="C19" s="0" t="n">
         <v>817424</v>
       </c>
-      <c r="D19" s="2" t="n">
+      <c r="D19" s="0" t="n">
         <v>344</v>
       </c>
-      <c r="E19" s="2" t="n">
+      <c r="E19" s="0" t="n">
         <v>5697329</v>
       </c>
-      <c r="F19" s="2" t="n">
+      <c r="F19" s="0" t="n">
         <v>405</v>
       </c>
-      <c r="G19" s="2" t="n">
+      <c r="G19" s="0" t="n">
         <v>6514753</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="B20" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C20" s="2" t="n">
+      <c r="C20" s="0" t="n">
         <v>146789</v>
       </c>
-      <c r="D20" s="2" t="n">
+      <c r="D20" s="0" t="n">
         <v>107</v>
       </c>
-      <c r="E20" s="2" t="n">
+      <c r="E20" s="0" t="n">
         <v>1761584</v>
       </c>
-      <c r="F20" s="2" t="n">
+      <c r="F20" s="0" t="n">
         <v>118</v>
       </c>
-      <c r="G20" s="2" t="n">
+      <c r="G20" s="0" t="n">
         <v>1908373</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="B21" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C21" s="2" t="n">
+      <c r="C21" s="0" t="n">
         <v>12252</v>
       </c>
-      <c r="D21" s="2" t="n">
+      <c r="D21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="E21" s="2" t="n">
+      <c r="E21" s="0" t="n">
         <v>203691</v>
       </c>
-      <c r="F21" s="2" t="n">
+      <c r="F21" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="G21" s="2" t="n">
+      <c r="G21" s="0" t="n">
         <v>215943</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B22" s="0" t="n">
         <v>1351</v>
       </c>
-      <c r="C22" s="2" t="n">
+      <c r="C22" s="0" t="n">
         <v>29989451</v>
       </c>
-      <c r="D22" s="2" t="n">
+      <c r="D22" s="0" t="n">
         <v>4028</v>
       </c>
-      <c r="E22" s="2" t="n">
+      <c r="E22" s="0" t="n">
         <v>104043913</v>
       </c>
-      <c r="F22" s="2" t="n">
+      <c r="F22" s="0" t="n">
         <v>5379</v>
       </c>
-      <c r="G22" s="2" t="n">
+      <c r="G22" s="0" t="n">
         <v>134033364</v>
       </c>
     </row>

</xml_diff>